<commit_message>
Added additional county, neighborhood, borough look up tables and code to deal with zip code as string (vs. num)
</commit_message>
<xml_diff>
--- a/Mentoring Data Columns.xlsx
+++ b/Mentoring Data Columns.xlsx
@@ -11,9 +11,10 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$K$150</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$J$147</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$K$149</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$A$1:$J$147</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$A$1:$K$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Sheet1!$A$1:$J$147</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="329">
   <si>
     <t xml:space="preserve">Columns</t>
   </si>
@@ -303,6 +304,9 @@
     <t xml:space="preserve">se_event_type_value</t>
   </si>
   <si>
+    <t xml:space="preserve">Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">se_event_type_desc</t>
   </si>
   <si>
@@ -546,9 +550,6 @@
     <t xml:space="preserve">cl_business_type_code</t>
   </si>
   <si>
-    <t xml:space="preserve">Code</t>
-  </si>
-  <si>
     <t xml:space="preserve">Client business type</t>
   </si>
   <si>
@@ -993,13 +994,25 @@
     <t xml:space="preserve">Firscal year &amp; quarter</t>
   </si>
   <si>
-    <t xml:space="preserve">county_name</t>
+    <t xml:space="preserve">county</t>
   </si>
   <si>
     <t xml:space="preserve">Feature Engineered</t>
   </si>
   <si>
-    <t xml:space="preserve">neighborhood</t>
+    <t xml:space="preserve">County (based on zip code prefix)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NY_neighborhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NY neighborhood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NY_borough</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NY Borough</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1053,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1057,6 +1070,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF00FF"/>
+        <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1100,7 +1119,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1149,18 +1168,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1171,6 +1178,26 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1254,12 +1281,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ149"/>
+  <dimension ref="A1:AMJ150"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="510" topLeftCell="A43" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="510" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H76" activeCellId="0" sqref="H76"/>
+      <selection pane="bottomLeft" activeCell="F133" activeCellId="0" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1274,7 +1301,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="30.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="38.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="23.08"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1454,13 +1481,13 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="12" t="s">
         <v>40</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="13" t="s">
         <v>41</v>
       </c>
       <c r="J13" s="0" t="s">
@@ -1564,7 +1591,7 @@
       <c r="H23" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="J23" s="14" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1575,7 +1602,7 @@
       <c r="H24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="J24" s="14" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1586,95 +1613,95 @@
       <c r="H25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="J25" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="H26" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J26" s="12" t="s">
+      <c r="H26" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J26" s="14" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="H27" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" s="12" t="s">
+      <c r="H27" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J27" s="14" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J28" s="12" t="s">
+      <c r="H28" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="14" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H29" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J29" s="12" t="s">
+      <c r="H29" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J29" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H30" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J30" s="12" t="s">
+      <c r="H30" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J30" s="14" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J31" s="12" t="s">
+      <c r="H31" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J31" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J32" s="12" t="s">
+      <c r="H32" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J32" s="14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="H33" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="J33" s="12" t="s">
+      <c r="H33" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="J33" s="14" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1685,7 +1712,7 @@
       <c r="H34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J34" s="12" t="s">
+      <c r="J34" s="14" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1696,7 +1723,7 @@
       <c r="H35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J35" s="12" t="s">
+      <c r="J35" s="14" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1707,7 +1734,7 @@
       <c r="H36" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J36" s="12" t="s">
+      <c r="J36" s="14" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1718,24 +1745,27 @@
       <c r="H37" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J37" s="12" t="s">
+      <c r="J37" s="14" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="H38" s="11" t="s">
-        <v>34</v>
+      <c r="H38" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>24</v>
@@ -1744,21 +1774,21 @@
         <v>4</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>17</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
-        <v>97</v>
+      <c r="A40" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>49</v>
@@ -1771,22 +1801,25 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>34</v>
+      <c r="A41" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="J41" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
-        <v>100</v>
+      <c r="A42" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>24</v>
@@ -1798,12 +1831,12 @@
         <v>17</v>
       </c>
       <c r="J42" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>49</v>
@@ -1817,7 +1850,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>49</v>
@@ -1831,7 +1864,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>49</v>
@@ -1845,23 +1878,23 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J46" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>24</v>
@@ -1870,12 +1903,12 @@
         <v>4</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>49</v>
@@ -1886,35 +1919,35 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D50" s="2" t="n">
         <v>2</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>49</v>
@@ -1925,7 +1958,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>49</v>
@@ -1936,7 +1969,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>49</v>
@@ -1947,7 +1980,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>49</v>
@@ -1955,23 +1988,23 @@
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>49</v>
@@ -1983,25 +2016,25 @@
         <v>2</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J58" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>49</v>
@@ -2012,17 +2045,17 @@
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="15" t="s">
-        <v>133</v>
+      <c r="A64" s="18" t="s">
+        <v>134</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>49</v>
@@ -2030,75 +2063,75 @@
       <c r="F64" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H64" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I64" s="16" t="s">
-        <v>134</v>
+      <c r="H64" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I64" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J64" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="H65" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" s="19" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="H65" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I65" s="16" t="s">
-        <v>134</v>
-      </c>
       <c r="J65" s="0" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="H66" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I66" s="16" t="s">
-        <v>134</v>
+      <c r="A66" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H66" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="H67" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I67" s="16" t="s">
-        <v>134</v>
+      <c r="A67" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="H67" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="H68" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I68" s="16" t="s">
-        <v>134</v>
+      <c r="A68" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I68" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J68" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="15" t="s">
-        <v>144</v>
+      <c r="A69" s="18" t="s">
+        <v>145</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>49</v>
@@ -2106,133 +2139,133 @@
       <c r="F69" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H69" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I69" s="16" t="s">
-        <v>134</v>
+      <c r="H69" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I69" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J69" s="0" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="H71" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I71" s="16" t="s">
-        <v>134</v>
+      <c r="A71" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="H71" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="H73" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I73" s="16" t="s">
-        <v>134</v>
+      <c r="A73" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="H73" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J73" s="0" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="H74" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I74" s="16" t="s">
-        <v>134</v>
+      <c r="A74" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="H74" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I74" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="H75" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="I75" s="18"/>
+      <c r="A75" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="H75" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I75" s="15"/>
       <c r="J75" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="H77" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I77" s="16" t="s">
-        <v>134</v>
+      <c r="A77" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="H77" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I77" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="H78" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I78" s="16" t="s">
-        <v>134</v>
+      <c r="A78" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="H78" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I78" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C80" s="0" t="s">
         <v>24</v>
@@ -2241,15 +2274,15 @@
         <v>5</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J80" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>49</v>
@@ -2261,29 +2294,29 @@
         <v>3</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>17</v>
       </c>
       <c r="J81" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J82" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="10" t="s">
-        <v>172</v>
+      <c r="A83" s="12" t="s">
+        <v>173</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>33</v>
@@ -2294,11 +2327,11 @@
       <c r="D83" s="2" t="n">
         <v>22</v>
       </c>
-      <c r="H83" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>173</v>
+      <c r="H83" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I83" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="J83" s="0" t="s">
         <v>174</v>
@@ -2328,7 +2361,7 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="10" t="s">
+      <c r="A85" s="12" t="s">
         <v>178</v>
       </c>
       <c r="B85" s="1" t="s">
@@ -2340,11 +2373,11 @@
       <c r="D85" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="H85" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>173</v>
+      <c r="H85" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I85" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="J85" s="0" t="s">
         <v>179</v>
@@ -2444,7 +2477,7 @@
         <v>49</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H90" s="2" t="s">
         <v>17</v>
@@ -2501,7 +2534,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="14" t="s">
+      <c r="A95" s="17" t="s">
         <v>202</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -2529,28 +2562,28 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="15" t="s">
+      <c r="A97" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="H97" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I97" s="16" t="s">
-        <v>134</v>
+      <c r="H97" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I97" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J97" s="0" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="15" t="s">
+      <c r="A98" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="H98" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I98" s="16" t="s">
-        <v>134</v>
+      <c r="H98" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I98" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J98" s="0" t="s">
         <v>209</v>
@@ -2687,7 +2720,7 @@
         <v>24</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G105" s="3" t="s">
         <v>227</v>
@@ -2713,7 +2746,7 @@
         <v>24</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G106" s="3" t="s">
         <v>227</v>
@@ -2721,7 +2754,7 @@
       <c r="H106" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J106" s="12" t="s">
+      <c r="J106" s="14" t="s">
         <v>228</v>
       </c>
       <c r="K106" s="0" t="s">
@@ -2822,7 +2855,7 @@
         <v>3</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H111" s="2" t="s">
         <v>17</v>
@@ -2845,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H112" s="2" t="s">
         <v>17</v>
@@ -2862,7 +2895,7 @@
         <v>49</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J113" s="0" t="s">
         <v>248</v>
@@ -2896,7 +2929,7 @@
         <v>49</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="J115" s="0" t="s">
         <v>253</v>
@@ -2908,17 +2941,17 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="15" t="s">
+      <c r="A117" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="H117" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="I117" s="16" t="s">
-        <v>134</v>
+      <c r="H117" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="I117" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="J117" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3142,7 +3175,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="10" t="s">
+      <c r="A138" s="16" t="s">
         <v>298</v>
       </c>
       <c r="C138" s="0" t="s">
@@ -3154,7 +3187,7 @@
       <c r="G138" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="H138" s="11" t="s">
+      <c r="H138" s="20" t="s">
         <v>34</v>
       </c>
       <c r="J138" s="0" t="s">
@@ -3264,16 +3297,42 @@
       <c r="A148" s="0" t="s">
         <v>322</v>
       </c>
+      <c r="C148" s="0" t="s">
+        <v>123</v>
+      </c>
       <c r="I148" s="2" t="s">
         <v>323</v>
       </c>
+      <c r="J148" s="0" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
+      </c>
+      <c r="C149" s="0" t="s">
+        <v>123</v>
       </c>
       <c r="I149" s="2" t="s">
         <v>323</v>
+      </c>
+      <c r="J149" s="0" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="C150" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="I150" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="J150" s="0" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reduced data by eliminating rows that contain zip code columns that are "NULL".  Recuded data with columns that are duplicate of another column or contain codes.  Also, reduced data excluding session type and event type that are not session related.
</commit_message>
<xml_diff>
--- a/Mentoring Data Columns.xlsx
+++ b/Mentoring Data Columns.xlsx
@@ -11,10 +11,12 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$K$150</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$K$147</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$J$147</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$A$1:$K$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$A$1:$K$150</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Sheet1!$A$1:$J$147</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">Sheet1!$A$1:$K$149</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$J$147</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="322">
   <si>
     <t xml:space="preserve">Columns</t>
   </si>
@@ -992,27 +994,6 @@
   </si>
   <si>
     <t xml:space="preserve">Firscal year &amp; quarter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">county</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Feature Engineered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">County (based on zip code prefix)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NY_neighborhood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NY neighborhood</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NY_borough</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NY Borough</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1100,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1184,10 +1165,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1197,10 +1174,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1281,12 +1254,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AMJ150"/>
+  <dimension ref="A1:AMJ147"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="510" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="510" topLeftCell="A127" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F133" activeCellId="0" sqref="F133"/>
+      <selection pane="bottomLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1787,7 +1760,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="14" t="s">
         <v>98</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1815,7 +1788,7 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>101</v>
       </c>
       <c r="B42" s="1" t="s">
@@ -2054,7 +2027,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="17" t="s">
         <v>134</v>
       </c>
       <c r="B64" s="1" t="s">
@@ -2063,10 +2036,10 @@
       <c r="F64" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H64" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I64" s="19" t="s">
+      <c r="H64" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I64" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J64" s="0" t="s">
@@ -2074,13 +2047,13 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="H65" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I65" s="19" t="s">
+      <c r="H65" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I65" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J65" s="0" t="s">
@@ -2088,13 +2061,13 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="H66" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I66" s="19" t="s">
+      <c r="H66" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I66" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J66" s="0" t="s">
@@ -2102,13 +2075,13 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="18" t="s">
+      <c r="A67" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="H67" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I67" s="19" t="s">
+      <c r="H67" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I67" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J67" s="0" t="s">
@@ -2116,13 +2089,13 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="18" t="s">
+      <c r="A68" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="H68" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I68" s="19" t="s">
+      <c r="H68" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I68" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J68" s="0" t="s">
@@ -2130,7 +2103,7 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="17" t="s">
         <v>145</v>
       </c>
       <c r="B69" s="1" t="s">
@@ -2139,10 +2112,10 @@
       <c r="F69" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H69" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I69" s="19" t="s">
+      <c r="H69" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I69" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J69" s="0" t="s">
@@ -2158,13 +2131,13 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="H71" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I71" s="19" t="s">
+      <c r="H71" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I71" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J71" s="0" t="s">
@@ -2180,13 +2153,13 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="H73" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I73" s="19" t="s">
+      <c r="H73" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I73" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J73" s="0" t="s">
@@ -2194,13 +2167,13 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="18" t="s">
+      <c r="A74" s="17" t="s">
         <v>154</v>
       </c>
-      <c r="H74" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I74" s="19" t="s">
+      <c r="H74" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I74" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J74" s="0" t="s">
@@ -2231,13 +2204,13 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="18" t="s">
+      <c r="A77" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="H77" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I77" s="19" t="s">
+      <c r="H77" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I77" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J77" s="0" t="s">
@@ -2245,13 +2218,13 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="18" t="s">
+      <c r="A78" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="H78" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I78" s="19" t="s">
+      <c r="H78" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I78" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J78" s="0" t="s">
@@ -2534,7 +2507,7 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="16" t="s">
         <v>202</v>
       </c>
       <c r="B95" s="1" t="s">
@@ -2562,13 +2535,13 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="18" t="s">
+      <c r="A97" s="17" t="s">
         <v>206</v>
       </c>
-      <c r="H97" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I97" s="19" t="s">
+      <c r="H97" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I97" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J97" s="0" t="s">
@@ -2576,13 +2549,13 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="18" t="s">
+      <c r="A98" s="17" t="s">
         <v>208</v>
       </c>
-      <c r="H98" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I98" s="19" t="s">
+      <c r="H98" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I98" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J98" s="0" t="s">
@@ -2941,13 +2914,13 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="H117" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I117" s="19" t="s">
+      <c r="H117" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I117" s="18" t="s">
         <v>135</v>
       </c>
       <c r="J117" s="0" t="s">
@@ -3175,7 +3148,7 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="16" t="s">
+      <c r="A138" s="14" t="s">
         <v>298</v>
       </c>
       <c r="C138" s="0" t="s">
@@ -3187,7 +3160,7 @@
       <c r="G138" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="H138" s="20" t="s">
+      <c r="H138" s="15" t="s">
         <v>34</v>
       </c>
       <c r="J138" s="0" t="s">
@@ -3291,48 +3264,6 @@
       </c>
       <c r="J147" s="0" t="s">
         <v>321</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="C148" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I148" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="J148" s="0" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="C149" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I149" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="J149" s="0" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="C150" s="0" t="s">
-        <v>123</v>
-      </c>
-      <c r="I150" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="J150" s="0" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>